<commit_message>
multiple table registration is now working. detail view all are dynamically generated. enabling and disabling beneficiary_entity_ids is working. delivery cannot be tested because setsublist lacks arbitrary query. split pane view is refactored into one file and is working.
</commit_message>
<xml_diff>
--- a/app/config/tables/authorization_reports/forms/authorization_reports/authorization_reports.xlsx
+++ b/app/config/tables/authorization_reports/forms/authorization_reports/authorization_reports.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/new_redcross_repos/redcross-app-designer/appGreece/config/tables/authorization_reports/forms/authorization_reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/new_redcross_repos/redcross-app-designer/app/config/tables/authorization_reports/forms/authorization_reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="460" windowWidth="28800" windowHeight="16220" tabRatio="994" activeTab="1"/>
+    <workbookView xWindow="5040" yWindow="460" windowWidth="28800" windowHeight="16220" tabRatio="994"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>type</t>
   </si>
@@ -101,18 +101,6 @@
     <t>authorization_id</t>
   </si>
   <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>Record any relevant notes on this distribution</t>
-  </si>
-  <si>
-    <t>admin_name</t>
-  </si>
-  <si>
-    <t>What is your name?</t>
-  </si>
-  <si>
     <t>user</t>
   </si>
   <si>
@@ -129,6 +117,12 @@
   </si>
   <si>
     <t>Authorization Reports</t>
+  </si>
+  <si>
+    <t>placeholder text</t>
+  </si>
+  <si>
+    <t>note</t>
   </si>
 </sst>
 </file>
@@ -748,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -767,7 +761,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>1</v>
@@ -785,11 +779,9 @@
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="B2" s="7"/>
       <c r="C2" s="11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="9"/>
@@ -798,15 +790,7 @@
       <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>23</v>
-      </c>
+      <c r="C3" s="11"/>
       <c r="D3" s="12"/>
       <c r="E3" s="9"/>
       <c r="F3" s="10"/>
@@ -1043,7 +1027,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1070,7 +1054,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C2"/>
     </row>
@@ -1088,7 +1072,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C4"/>
     </row>
@@ -1098,7 +1082,7 @@
       </c>
       <c r="B5"/>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1144,7 +1128,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1152,7 +1136,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1160,7 +1144,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1168,7 +1152,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>